<commit_message>
ability to join participant tables in research/participants table.
</commit_message>
<xml_diff>
--- a/emma_backend/research/participants/PTable2.xlsx
+++ b/emma_backend/research/participants/PTable2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Gerontechnology\emma_backend\research\participants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EAEF9B-30B9-4E7A-B849-4833DD9F8CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770E1D36-D07E-43D0-B89F-5089857B156C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,19 +120,19 @@
     <t>bb765</t>
   </si>
   <si>
+    <t>participant_name</t>
+  </si>
+  <si>
+    <t>study</t>
+  </si>
+  <si>
+    <t>cohort</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
     <t>participant_id</t>
-  </si>
-  <si>
-    <t>participant_name</t>
-  </si>
-  <si>
-    <t>study</t>
-  </si>
-  <si>
-    <t>cohort</t>
-  </si>
-  <si>
-    <t>active</t>
   </si>
 </sst>
 </file>
@@ -460,27 +460,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>34</v>
-      </c>
-      <c r="E1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>